<commit_message>
add solo titles dungeon bomb balloon sort
</commit_message>
<xml_diff>
--- a/data/rival.xlsx
+++ b/data/rival.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/94468aa6da851130/Desktop/reto/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="621" documentId="8_{9713198C-5AF7-4EEE-B6B7-339E279726B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FFE4F83-118C-47A1-9167-CAAD1A5B5050}"/>
+  <xr:revisionPtr revIDLastSave="663" documentId="8_{9713198C-5AF7-4EEE-B6B7-339E279726B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8791987D-2962-45D3-A391-39F64400638A}"/>
   <bookViews>
-    <workbookView xWindow="5535" yWindow="2985" windowWidth="11505" windowHeight="12210" xr2:uid="{610C4827-A39E-4D77-86AB-FDE647078AA6}"/>
+    <workbookView xWindow="2130" yWindow="2430" windowWidth="12345" windowHeight="12885" xr2:uid="{610C4827-A39E-4D77-86AB-FDE647078AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>player</t>
     <phoneticPr fontId="1"/>
@@ -571,6 +571,30 @@
     <t>オートキュイジーヌ卿</t>
     <rPh sb="9" eb="10">
       <t>キョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>無法者集団</t>
+    <rPh sb="0" eb="5">
+      <t>ムホウモノシュウダン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最高戦力</t>
+    <rPh sb="0" eb="2">
+      <t>サイコウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>センリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>知識王</t>
+    <rPh sb="0" eb="3">
+      <t>チシキオウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -961,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CB0C30-A935-445D-8022-3321E6129271}">
-  <dimension ref="A1:J82"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3597,6 +3621,102 @@
         <v>257</v>
       </c>
     </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83">
+        <v>2400</v>
+      </c>
+      <c r="C83">
+        <v>9999</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
+        <v>10</v>
+      </c>
+      <c r="F83">
+        <v>10001</v>
+      </c>
+      <c r="G83">
+        <v>944</v>
+      </c>
+      <c r="H83">
+        <v>270</v>
+      </c>
+      <c r="I83">
+        <v>996</v>
+      </c>
+      <c r="J83">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84">
+        <v>2400</v>
+      </c>
+      <c r="C84">
+        <v>9999</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>10</v>
+      </c>
+      <c r="F84">
+        <v>830</v>
+      </c>
+      <c r="G84">
+        <v>357</v>
+      </c>
+      <c r="H84">
+        <v>595</v>
+      </c>
+      <c r="I84">
+        <v>538</v>
+      </c>
+      <c r="J84">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85">
+        <v>2400</v>
+      </c>
+      <c r="C85">
+        <v>9999</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85">
+        <v>10</v>
+      </c>
+      <c r="F85">
+        <v>1076</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85">
+        <v>3</v>
+      </c>
+      <c r="J85">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>